<commit_message>
Fix capital letter bug during test generation
</commit_message>
<xml_diff>
--- a/examples/hu.bme.mit.gamma.railway.casestudy/measurements/test-generation.xlsx
+++ b/examples/hu.bme.mit.gamma.railway.casestudy/measurements/test-generation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B\git\gamma\examples\hu.bme.mit.gamma.railway.casestudy\measurements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED4816C-DDCF-4F0A-B404-FE6BDABE3C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5F9FE1-C6BA-477B-8158-32B4A6761187}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -434,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="J111" sqref="J111"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A97" sqref="A97:E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -999,47 +999,47 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>164.50747459999999</v>
+        <v>100.31432100000001</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>163.93065279999999</v>
+        <v>99.183032400000002</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>165.2445381</v>
+        <v>99.652045700000002</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
-        <v>164.64172640000001</v>
+        <v>99.072445900000005</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
-        <v>164.493977</v>
+        <v>98.563304400000007</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
-        <v>164.5738437</v>
+        <v>98.675149200000007</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
-        <v>164.0300905</v>
+        <v>99.273589299999998</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
-        <v>160.84863469999999</v>
+        <v>98.672026900000006</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
-        <v>163.83466949999999</v>
+        <v>98.5674578</v>
       </c>
       <c r="C106" t="s">
         <v>23</v>
@@ -1050,15 +1050,15 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
-        <v>164.8612133</v>
+        <v>98.670061799999999</v>
       </c>
       <c r="C107">
         <f>AVERAGE(A98:A107)</f>
-        <v>164.09668205999998</v>
+        <v>99.064343439999988</v>
       </c>
       <c r="D107">
         <f>MEDIAN(A98:A107)</f>
-        <v>164.5007258</v>
+        <v>98.873797550000006</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
@@ -1068,47 +1068,47 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
-        <v>106.4933393</v>
+        <v>87.6078665</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
-        <v>106.7557413</v>
+        <v>87.518438099999997</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
-        <v>106.84208940000001</v>
+        <v>87.390573200000006</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
-        <v>106.9404775</v>
+        <v>86.6157003</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
-        <v>109.25935130000001</v>
+        <v>86.693950099999995</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
-        <v>108.2510589</v>
+        <v>87.434033799999995</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
-        <v>107.2732481</v>
+        <v>86.6610522</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
-        <v>107.2025316</v>
+        <v>86.401674600000007</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
-        <v>107.1828706</v>
+        <v>87.029958699999995</v>
       </c>
       <c r="C118" t="s">
         <v>23</v>
@@ -1119,15 +1119,15 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
-        <v>107.6073914</v>
+        <v>87.241060899999994</v>
       </c>
       <c r="C119">
         <f>AVERAGE(A110:A119)</f>
-        <v>107.38080994000002</v>
+        <v>87.059430839999976</v>
       </c>
       <c r="D119">
         <f>MEDIAN(A110:A119)</f>
-        <v>107.19270109999999</v>
+        <v>87.135509799999994</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
@@ -1709,47 +1709,47 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225">
-        <v>100.31432100000001</v>
+        <v>164.50747459999999</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226">
-        <v>99.183032400000002</v>
+        <v>163.93065279999999</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227">
-        <v>99.652045700000002</v>
+        <v>165.2445381</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228">
-        <v>99.072445900000005</v>
+        <v>164.64172640000001</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229">
-        <v>98.563304400000007</v>
+        <v>164.493977</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230">
-        <v>98.675149200000007</v>
+        <v>164.5738437</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231">
-        <v>99.273589299999998</v>
+        <v>164.0300905</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232">
-        <v>98.672026900000006</v>
+        <v>160.84863469999999</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233">
-        <v>98.5674578</v>
+        <v>163.83466949999999</v>
       </c>
       <c r="C233" t="s">
         <v>23</v>
@@ -1760,15 +1760,15 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234">
-        <v>98.670061799999999</v>
+        <v>164.8612133</v>
       </c>
       <c r="C234">
         <f>AVERAGE(A225:A234)</f>
-        <v>99.064343439999988</v>
+        <v>164.09668205999998</v>
       </c>
       <c r="D234">
         <f>MEDIAN(A225:A234)</f>
-        <v>98.873797550000006</v>
+        <v>164.5007258</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.3">
@@ -1778,47 +1778,47 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237">
-        <v>87.6078665</v>
+        <v>106.4933393</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238">
-        <v>87.518438099999997</v>
+        <v>106.7557413</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239">
-        <v>87.390573200000006</v>
+        <v>106.84208940000001</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240">
-        <v>86.6157003</v>
+        <v>106.9404775</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241">
-        <v>86.693950099999995</v>
+        <v>109.25935130000001</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242">
-        <v>87.434033799999995</v>
+        <v>108.2510589</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243">
-        <v>86.6610522</v>
+        <v>107.2732481</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244">
-        <v>86.401674600000007</v>
+        <v>107.2025316</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245">
-        <v>87.029958699999995</v>
+        <v>107.1828706</v>
       </c>
       <c r="C245" t="s">
         <v>23</v>
@@ -1829,15 +1829,15 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246">
-        <v>87.241060899999994</v>
+        <v>107.6073914</v>
       </c>
       <c r="C246">
         <f>AVERAGE(A237:A246)</f>
-        <v>87.059430839999976</v>
+        <v>107.38080994000002</v>
       </c>
       <c r="D246">
         <f>MEDIAN(A237:A246)</f>
-        <v>87.135509799999994</v>
+        <v>107.19270109999999</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>